<commit_message>
styling and fixing bug
</commit_message>
<xml_diff>
--- a/input/questions.xlsx
+++ b/input/questions.xlsx
@@ -67,13 +67,13 @@
     <t xml:space="preserve">GIF4_Q3_Parrot.gif</t>
   </si>
   <si>
-    <t xml:space="preserve">You quickly turn down the volume of the espresso machine and provide a cozy corner for them</t>
+    <t xml:space="preserve">You quickly turn down the volume of the espresso machine and provide a cozy corner for them.</t>
   </si>
   <si>
     <t xml:space="preserve">Responsive</t>
   </si>
   <si>
-    <t xml:space="preserve">You provide toys and treats to keep the parrot entertained so the customer can enjoy their coffee</t>
+    <t xml:space="preserve">You provide toys and treats to keep the parrot entertained so the customer can enjoy their coffee.</t>
   </si>
   <si>
     <t xml:space="preserve">You notice a shy customer struggling to decide on a drink. </t>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">GIF5_Q4_Shy.gif</t>
   </si>
   <si>
-    <t xml:space="preserve">You provide detailed descriptions of both menu options to help them decide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You wait patiently and assure them that many customers also struggle to decide on their order</t>
+    <t xml:space="preserve">You provide detailed descriptions of both menu options to help them decide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You wait patiently and assure them that many customers also struggle to decide on their order.</t>
   </si>
   <si>
     <t xml:space="preserve">Empathetic</t>
@@ -97,10 +97,10 @@
     <t xml:space="preserve">GIF6_Q5_MovieStar.gif</t>
   </si>
   <si>
-    <t xml:space="preserve">You approach the movie star discreetly and ask if he/she requires any assistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You respect their desire for privacy and ensure their visit remains low-key</t>
+    <t xml:space="preserve">You approach the movie star discreetly and ask if he/she requires any assistance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You respect their desire for privacy and ensure their visit remains low-key.</t>
   </si>
   <si>
     <t xml:space="preserve">Professional</t>
@@ -112,10 +112,10 @@
     <t xml:space="preserve">GIF7_Q6_50years.gif</t>
   </si>
   <si>
-    <t xml:space="preserve">You suggest a giant cookie cake adorned with heartfelt messages for each other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You suggest a tall cookie tower elegantly arranged to celebrate their special occasion</t>
+    <t xml:space="preserve">You suggest a giant cookie cake adorned with heartfelt messages for each other.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You suggest a tall cookie tower elegantly arranged to celebrate their special occasion.</t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -262,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,9 +271,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="91.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="98.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changed pictures and load strategy
</commit_message>
<xml_diff>
--- a/input/questions.xlsx
+++ b/input/questions.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">The cafe introduces a new drink called "Mystery Coffee". You were asked to describe it on the menuboard: </t>
   </si>
   <si>
-    <t xml:space="preserve">GIF3_Q2_MysteryDrink.gif</t>
+    <t xml:space="preserve">3.gif</t>
   </si>
   <si>
     <t xml:space="preserve">"Handcrafted by our expert baristas, made with exquisite coffee beans for an intriguing taste."</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">A regular customer brings in their pet parrot, who starts mimicking the sound of the espresso machine loudly. </t>
   </si>
   <si>
-    <t xml:space="preserve">GIF4_Q3_Parrot.gif</t>
+    <t xml:space="preserve">4.gif</t>
   </si>
   <si>
     <t xml:space="preserve">You quickly turn down the volume of the espresso machine and provide a cozy corner for them.</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">You notice a shy customer struggling to decide on a drink. </t>
   </si>
   <si>
-    <t xml:space="preserve">GIF5_Q4_Shy.gif</t>
+    <t xml:space="preserve">5.gif</t>
   </si>
   <si>
     <t xml:space="preserve">You provide detailed descriptions of both menu options to help them decide.</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">You spot a retired movie star seated discreetly at one corner of the cafe.</t>
   </si>
   <si>
-    <t xml:space="preserve">GIF6_Q5_MovieStar.gif</t>
+    <t xml:space="preserve">6.gif</t>
   </si>
   <si>
     <t xml:space="preserve">You approach the movie star discreetly and ask if he/she requires any assistance.</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">A group of grannies asks for a "monster-sized cookie cake" to celebrate 50 years of friendship.</t>
   </si>
   <si>
-    <t xml:space="preserve">GIF7_Q6_50years.gif</t>
+    <t xml:space="preserve">7.gif</t>
   </si>
   <si>
     <t xml:space="preserve">You suggest a giant cookie cake adorned with heartfelt messages for each other.</t>
@@ -262,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,9 +271,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="91.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="91.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="98.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="98.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.15"/>
   </cols>
   <sheetData>

</xml_diff>